<commit_message>
Ajuste con factor de correcion
</commit_message>
<xml_diff>
--- a/data/Evento_2/Potencial de aforo.xlsx
+++ b/data/Evento_2/Potencial de aforo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juank\turismo-religioso-analisis\data\Evento_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246B5D43-D10B-4F53-989C-73CB08A3CE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE80BA26-BBD9-4FA0-8287-5C4E07C1F93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7548" yWindow="3276" windowWidth="12288" windowHeight="11364" xr2:uid="{A83A83DE-78B3-4331-B8A6-038E19923D60}"/>
+    <workbookView xWindow="-26235" yWindow="2910" windowWidth="24645" windowHeight="11835" xr2:uid="{A83A83DE-78B3-4331-B8A6-038E19923D60}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -422,15 +422,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -446,12 +446,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5000</v>
+        <v>7000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>